<commit_message>
+ Update age cal
</commit_message>
<xml_diff>
--- a/Selenium_Test_C#/bin/Debug/Testcase_Age_Calculator.xlsx
+++ b/Selenium_Test_C#/bin/Debug/Testcase_Age_Calculator.xlsx
@@ -24,37 +24,37 @@
     <t>Jan</t>
   </si>
   <si>
-    <t>Error: Date of birth needs to be earlier than the age at date.</t>
-  </si>
-  <si>
     <t>Feb</t>
-  </si>
-  <si>
-    <t>Age:\n1 years 1 months 14 days\nor 13 months 14 days\nor 58 weeks 5 days\nor 411 days\nor 9,864 hours\nor 591,840 minutes\nor 35,510,400 seconds</t>
-  </si>
-  <si>
-    <t>Age:\n1 years 1 months 0 days\nor 13 months 0 days\nor 56 weeks 5 days\nor 397 days\nor 9,528 hours\nor 571,680 minutes\nor 34,300,800 seconds</t>
-  </si>
-  <si>
-    <t>Age:\n11 months 18 days\nor 50 weeks 3 days\nor 353 days\nor 8,472 hours\nor 508,320 minutes\nor 30,499,200 seconds</t>
-  </si>
-  <si>
-    <t>Age:\n1 years 0 months 0 days\nor 12 months 0 days\nor 52 weeks 2 days\nor 366 days\nor 8,784 hours\nor 527,040 minutes\nor 31,622,400 seconds</t>
   </si>
   <si>
     <t>Jul</t>
   </si>
   <si>
-    <t>Age:\n1 months 9 days\nor 5 weeks 5 days\nor 40 days\nor 960 hours\nor 57,600 minutes\nor 3,456,000 seconds</t>
+    <t>Date of birth needs to be earlier than the age at date.</t>
   </si>
   <si>
-    <t>Age:\n1 months 0 days\nor 4 weeks 3 days\nor 31 days\nor 744 hours\nor 44,640 minutes\nor 2,678,400 seconds</t>
+    <t>Age:1 years 1 months 14 daysor 13 months 14 daysor 58 weeks 5 daysor 411 daysor 9,864 hoursor 591,840 minutesor 35,510,400 seconds</t>
   </si>
   <si>
-    <t>Age:\n0 days\nor 0 hours\nor 0 minutes\nor 0 seconds</t>
+    <t>Age:1 years 1 months 0 daysor 13 months 0 daysor 56 weeks 5 daysor 397 daysor 9,528 hoursor 571,680 minutesor 34,300,800 seconds</t>
   </si>
   <si>
-    <t>Age:\n1 weeks 2 days\nor 9 days\nor 216 hours\nor 12,960 minutes\nor 777,600 seconds</t>
+    <t>Age:11 months 18 daysor 50 weeks 3 daysor 353 daysor 8,472 hoursor 508,320 minutesor 30,499,200 seconds</t>
+  </si>
+  <si>
+    <t>Age:1 years 0 months 0 daysor 12 months 0 daysor 52 weeks 2 daysor 366 daysor 8,784 hoursor 527,040 minutesor 31,622,400 seconds</t>
+  </si>
+  <si>
+    <t>Age:1 months 9 daysor 5 weeks 5 daysor 40 daysor 960 hoursor 57,600 minutesor 3,456,000 seconds</t>
+  </si>
+  <si>
+    <t>Age:1 months 0 daysor 4 weeks 3 daysor 31 daysor 744 hoursor 44,640 minutesor 2,678,400 seconds</t>
+  </si>
+  <si>
+    <t>Age:0 daysor 0 hoursor 0 minutesor 0 seconds</t>
+  </si>
+  <si>
+    <t>Age:1 weeks 2 daysor 9 daysor 216 hoursor 12,960 minutesor 777,600 seconds</t>
   </si>
 </sst>
 </file>
@@ -871,7 +871,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +896,7 @@
         <v>2000</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>2001</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -919,7 +919,7 @@
         <v>2000</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>2000</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,7 +956,7 @@
         <v>2001</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -965,7 +965,7 @@
         <v>2000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>2000</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -988,7 +988,7 @@
         <v>2001</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
         <v>2000</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>15</v>
@@ -1011,7 +1011,7 @@
         <v>2001</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
         <v>2001</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1057,12 +1057,12 @@
         <v>2001</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -1071,7 +1071,7 @@
         <v>2000</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1080,12 +1080,12 @@
         <v>2000</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1094,7 +1094,7 @@
         <v>2000</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1103,7 +1103,7 @@
         <v>2000</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1117,7 +1117,7 @@
         <v>2000</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1140,7 +1140,7 @@
         <v>2000</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1172,7 +1172,7 @@
         <v>2000</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>